<commit_message>
added notes on excel sheet
</commit_message>
<xml_diff>
--- a/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
+++ b/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
@@ -3011,6 +3011,80 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8658225" y="781050"/>
+          <a:ext cx="5962650" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>So we need to keep making the list of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> all the addresses of the companies on the Distant Company List (right now its all our companies). Once we have the list that has been started on the local company tab, we can filter out anything that is more then 20 minutes away and put it into the Distant Company sheet. The local companies will be visited in person with the sponsorship package by 2 SEDS members, and the distant companies will be emailed. This will all happen by the end of next week! </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:J210" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B1:J210"/>
@@ -7158,7 +7232,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7166,7 +7240,7 @@
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="83.42578125" customWidth="1"/>
     <col min="5" max="5" width="48.28515625" customWidth="1"/>
     <col min="6" max="6" width="76.42578125" customWidth="1"/>
     <col min="7" max="7" width="169" bestFit="1" customWidth="1"/>
@@ -8515,8 +8589,9 @@
     <hyperlink ref="C9" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
went to two companies
need to email goss to set up an appointment
</commit_message>
<xml_diff>
--- a/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
+++ b/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\UNHSEDS\Business\Finance\Sponsorship\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="848">
   <si>
     <t>Company Name</t>
   </si>
@@ -2642,7 +2642,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2655,8 +2655,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2688,12 +2694,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2751,23 +2770,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2833,6 +2857,17 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3278,30 +3313,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D70" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D70" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:D70"/>
   <sortState ref="A2:C69">
     <sortCondition ref="A1:A70"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Company Name" dataDxfId="10"/>
-    <tableColumn id="2" name="Address" dataDxfId="9"/>
-    <tableColumn id="3" name="Phone Number" dataDxfId="8"/>
-    <tableColumn id="4" name="Email" dataDxfId="7"/>
+    <tableColumn id="1" name="Company Name" dataDxfId="9"/>
+    <tableColumn id="2" name="Address" dataDxfId="8"/>
+    <tableColumn id="3" name="Phone Number" dataDxfId="7"/>
+    <tableColumn id="4" name="Email" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E25" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E25" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E25"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Company Name" dataDxfId="5"/>
-    <tableColumn id="2" name="Address" dataDxfId="4"/>
-    <tableColumn id="3" name="Number" dataDxfId="3"/>
-    <tableColumn id="4" name="Email" dataDxfId="2"/>
-    <tableColumn id="5" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" name="Company Name" dataDxfId="4"/>
+    <tableColumn id="2" name="Address" dataDxfId="3"/>
+    <tableColumn id="3" name="Number" dataDxfId="2"/>
+    <tableColumn id="4" name="Email" dataDxfId="1"/>
+    <tableColumn id="5" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9706,10 +9741,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9900,14 +9935,14 @@
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="32" t="s">
         <v>283</v>
       </c>
       <c r="E15" s="16"/>
@@ -10049,6 +10084,74 @@
         <v>30</v>
       </c>
       <c r="E25" s="16"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>736</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>735</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>824</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>644</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>839</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>709</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>734</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="11" t="s">
+        <v>246</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
solidworks hybrid first draft
</commit_message>
<xml_diff>
--- a/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
+++ b/Business/Finance/Sponsorship/Companies 2018-2019.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="851">
   <si>
     <t>Company Name</t>
   </si>
@@ -2583,6 +2583,15 @@
       </rPr>
       <t>230 Commerce Way #302, Portsmouth, NH 03801</t>
     </r>
+  </si>
+  <si>
+    <t>Notes, Who Went</t>
+  </si>
+  <si>
+    <t>Silas and Charlie, took PDF. Grace should follow up soon.</t>
+  </si>
+  <si>
+    <t>Need to set an appointment over phone or online</t>
   </si>
 </sst>
 </file>
@@ -3336,7 +3345,7 @@
     <tableColumn id="2" name="Address" dataDxfId="3"/>
     <tableColumn id="3" name="Number" dataDxfId="2"/>
     <tableColumn id="4" name="Email" dataDxfId="1"/>
-    <tableColumn id="5" name="Column1" dataDxfId="0"/>
+    <tableColumn id="5" name="Notes, Who Went" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9744,7 +9753,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9752,8 +9761,8 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9770,7 +9779,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>848</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9945,7 +9954,9 @@
       <c r="D15" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="16" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -10086,16 +10097,10 @@
       <c r="E25" s="16"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>736</v>
-      </c>
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="27"/>
-      <c r="D30" s="10" t="s">
-        <v>283</v>
-      </c>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
@@ -10107,6 +10112,9 @@
       <c r="C31" s="27"/>
       <c r="D31" s="11" t="s">
         <v>252</v>
+      </c>
+      <c r="E31" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>